<commit_message>
All 4 years scope emissions added.
</commit_message>
<xml_diff>
--- a/data/Nabers_3_Star.xlsx
+++ b/data/Nabers_3_Star.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashut\co-perform\Done_Archivede_future-improve\Nabers_calculator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ashut\co-perform\Git_repo\Nabers_calculator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9589021-CC7D-4061-956E-FBBFE2F9D775}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303ABACB-3307-4518-90E4-E3C3A4673B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,29 +33,23 @@
     <t>Hours</t>
   </si>
   <si>
-    <t>Target Max Electricity kWh per anum</t>
+    <t>Star Rating</t>
   </si>
   <si>
-    <t>Star Rating</t>
+    <t>emissions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF4A4A4A"/>
-      <name val="Verdana"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,7 +74,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -364,7 +358,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -377,10 +371,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -391,7 +385,7 @@
         <v>40</v>
       </c>
       <c r="C2" s="1">
-        <v>106021</v>
+        <v>115563.1</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -405,7 +399,7 @@
         <v>50</v>
       </c>
       <c r="C3" s="1">
-        <v>122776</v>
+        <v>133826.70000000001</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -419,7 +413,7 @@
         <v>60</v>
       </c>
       <c r="C4" s="1">
-        <v>139532</v>
+        <v>152090.4</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -433,7 +427,7 @@
         <v>40</v>
       </c>
       <c r="C5" s="1">
-        <v>212042</v>
+        <v>231126.2</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -447,7 +441,7 @@
         <v>50</v>
       </c>
       <c r="C6" s="1">
-        <v>245553</v>
+        <v>267653.5</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -461,7 +455,7 @@
         <v>60</v>
       </c>
       <c r="C7" s="1">
-        <v>279064</v>
+        <v>304180.8</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -475,7 +469,7 @@
         <v>40</v>
       </c>
       <c r="C8" s="1">
-        <v>318063</v>
+        <v>346689.2</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -489,7 +483,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="1">
-        <v>368330</v>
+        <v>401480.2</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -503,7 +497,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="1">
-        <v>418597</v>
+        <v>456271.1</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -517,7 +511,7 @@
         <v>40</v>
       </c>
       <c r="C11" s="1">
-        <v>424084</v>
+        <v>462252.3</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -531,7 +525,7 @@
         <v>50</v>
       </c>
       <c r="C12" s="1">
-        <v>491107</v>
+        <v>535306.9</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -545,7 +539,7 @@
         <v>60</v>
       </c>
       <c r="C13" s="1">
-        <v>558129</v>
+        <v>608361.5</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -559,7 +553,7 @@
         <v>40</v>
       </c>
       <c r="C14" s="1">
-        <v>530105</v>
+        <v>577815.4</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -573,7 +567,7 @@
         <v>50</v>
       </c>
       <c r="C15" s="1">
-        <v>613884</v>
+        <v>669133.6</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -587,7 +581,7 @@
         <v>60</v>
       </c>
       <c r="C16" s="1">
-        <v>697662</v>
+        <v>760451.9</v>
       </c>
       <c r="D16">
         <v>3</v>

</xml_diff>